<commit_message>
able to multi accounts
</commit_message>
<xml_diff>
--- a/TopicsVisualization/101相关用户微博id_3(带名字版）.xlsx
+++ b/TopicsVisualization/101相关用户微博id_3(带名字版）.xlsx
@@ -251,15 +251,22 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -273,21 +280,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -295,29 +288,30 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -340,47 +334,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -396,7 +350,53 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -404,6 +404,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -418,13 +425,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -442,31 +521,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -478,25 +545,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -508,13 +563,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -526,79 +605,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -612,12 +619,25 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -639,6 +659,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -655,8 +690,10 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -667,36 +704,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -717,149 +724,149 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -873,6 +880,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1197,7 +1207,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="E22" sqref="E14 E15 E16 E17 E18 E19 E20 E21 E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
@@ -1231,7 +1241,7 @@
       <c r="D1" s="4">
         <v>2617143030</v>
       </c>
-      <c r="E1" s="4">
+      <c r="E1" s="5">
         <v>6201247478</v>
       </c>
       <c r="F1" s="4">
@@ -1251,7 +1261,7 @@
       <c r="D2" s="4">
         <v>3670570930</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="5">
         <v>1674561030</v>
       </c>
       <c r="F2" s="4">
@@ -1271,7 +1281,7 @@
       <c r="D3" s="4">
         <v>5866685410</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="5">
         <v>5887213624</v>
       </c>
       <c r="F3" s="4">
@@ -1291,7 +1301,7 @@
       <c r="D4" s="4">
         <v>6540414301</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="5">
         <v>5951606667</v>
       </c>
       <c r="F4" s="4">
@@ -1311,7 +1321,7 @@
       <c r="D5" s="4">
         <v>5373966624</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="5">
         <v>6533408548</v>
       </c>
       <c r="F5" s="4">
@@ -1331,7 +1341,7 @@
       <c r="D6" s="4">
         <v>6514492322</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="5">
         <v>3030398737</v>
       </c>
       <c r="F6" s="4">
@@ -1367,7 +1377,7 @@
       <c r="D8" s="4">
         <v>5596094365</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="5">
         <v>2660385853</v>
       </c>
       <c r="F8" s="4">
@@ -1387,7 +1397,7 @@
       <c r="D9" s="4">
         <v>5572995980</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="5">
         <v>3126342443</v>
       </c>
       <c r="F9" s="4"/>
@@ -1405,7 +1415,7 @@
       <c r="D10" s="4">
         <v>6320649994</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="5">
         <v>2959869817</v>
       </c>
       <c r="F10" s="4">
@@ -1425,7 +1435,7 @@
       <c r="D11" s="4">
         <v>5230206777</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="5">
         <v>5392529186</v>
       </c>
       <c r="F11" s="4">
@@ -1445,7 +1455,7 @@
       <c r="D12" s="4">
         <v>6512765246</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="5">
         <v>2003722997</v>
       </c>
       <c r="F12" s="4"/>
@@ -1463,7 +1473,7 @@
       <c r="D13" s="4">
         <v>5664160575</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="5">
         <v>6391488795</v>
       </c>
       <c r="F13" s="4"/>

</xml_diff>